<commit_message>
updated the hybrid framework
</commit_message>
<xml_diff>
--- a/exceltestdata/TC003.xlsx
+++ b/exceltestdata/TC003.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\eclipse-workspace\MavenProject\exceltestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B620AC1-2F59-4E05-963B-A7DD2A3AA24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D856F16-413A-4CF8-9E39-0961ADA49BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>AccountTitle</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>Salesforce Automation by  Sankarakarthikeyan</t>
-  </si>
-  <si>
-    <t>VerifyText</t>
-  </si>
-  <si>
-    <t>No items to display.</t>
   </si>
   <si>
     <t>UserName</t>
@@ -380,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,46 +385,37 @@
     <col min="3" max="3" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>